<commit_message>
Resource model add Javassist
</commit_message>
<xml_diff>
--- a/static-resource/configValueResource.xlsx
+++ b/static-resource/configValueResource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsonp/Documents/GitHub/netty-game-server/static-resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9264F4C-4A76-A143-83A5-8BA9E29E4547}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37062AC2-4A98-6649-84CA-C12A614F3D6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="900" windowWidth="28160" windowHeight="15880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>configValue</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>{1}</t>
+  </si>
+  <si>
+    <t>数据类型</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>数据class</t>
+  </si>
+  <si>
+    <t>clz</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>OBJECT</t>
+  </si>
+  <si>
+    <t>ARRAY</t>
   </si>
 </sst>
 </file>
@@ -409,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -421,12 +442,12 @@
     <col min="3" max="3" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -436,8 +457,14 @@
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -447,8 +474,14 @@
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -458,8 +491,14 @@
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -469,8 +508,14 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -479,6 +524,12 @@
       </c>
       <c r="C6" t="s">
         <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>